<commit_message>
Unit test cases added
</commit_message>
<xml_diff>
--- a/Docs/UTC_Survey.xlsx
+++ b/Docs/UTC_Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anshif\Projects\Survey\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B78494-3100-48EA-BFE3-01B8BC69A963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC6C3BB-B2E1-4100-9AF7-69A06BF75745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,122 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Sl No</t>
   </si>
   <si>
-    <t>Test Case</t>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Result (Pass/Fail)</t>
+  </si>
+  <si>
+    <t>Test API</t>
+  </si>
+  <si>
+    <t>fetch initial survey list</t>
+  </si>
+  <si>
+    <t>empty list with 200 http code</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>POST : http://localhost:8084/survey-service/api/admin/survey</t>
+  </si>
+  <si>
+    <t>GET :  http://localhost:8084/survey-service/api/admin/survey</t>
+  </si>
+  <si>
+    <t>Create first survey with name and description</t>
+  </si>
+  <si>
+    <t>Should create the survey in DB and return success status</t>
+  </si>
+  <si>
+    <t>Get the created survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET : http://localhost:8084/survey-service/api/admin/survey/question </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST : http://localhost:8084/survey-service/api/admin/survey/question </t>
+  </si>
+  <si>
+    <t>Should fetch the survey with id = 1</t>
+  </si>
+  <si>
+    <t>fetch questions for the created survey with id = 1</t>
+  </si>
+  <si>
+    <t>Should add the question to the curresponding survey</t>
+  </si>
+  <si>
+    <t>Add a new question and options to the survey with id = 1</t>
+  </si>
+  <si>
+    <t>fetch the added question and answers for the survey with id = 1</t>
+  </si>
+  <si>
+    <t>Should fetch all the questions and answers added to the survey</t>
+  </si>
+  <si>
+    <t>Create a survey with existing survey name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "status": "FAILED",
+    "code": "406",
+    "message": "The survey already exists"</t>
+  </si>
+  <si>
+    <t>Add a new question and options to an invalid survey id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "status": "FAILED",
+    "code": "500",
+    "message": "Failed to created the question."</t>
+  </si>
+  <si>
+    <t>GET : http://localhost:8084/survey-service/api/customer/questionnaire</t>
+  </si>
+  <si>
+    <t>Get the questionnaire for survey id = 1 and username = usr1</t>
+  </si>
+  <si>
+    <t>Should fetch a new questionnaire</t>
+  </si>
+  <si>
+    <t>POST : http://localhost:8084/survey-service/api/customer/questionnaire</t>
+  </si>
+  <si>
+    <t>Save the questionnaire with 'In Progress' status and selected options</t>
+  </si>
+  <si>
+    <t>Should create a new questionnaire in DB with 'In Progress' status</t>
+  </si>
+  <si>
+    <t>Should fetch the In-Progress questionnaire and already saved answers</t>
+  </si>
+  <si>
+    <t>Submit the questionnaire with 'Completed' status and selected options</t>
+  </si>
+  <si>
+    <t>Should update the questionnaire in DB with 'Completed' status</t>
+  </si>
+  <si>
+    <t>Should fetch completed status for the questionnaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +148,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,14 +185,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,26 +500,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" customWidth="1"/>
+    <col min="2" max="2" width="65.21875" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://localhost:8084/survey-service/api/admin/survey" xr:uid="{58CC83F4-0FC6-4A6B-BCA0-3051C0751AF9}"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://localhost:8084/survey-service/api/admin/survey" xr:uid="{7CA06CF5-02BA-44E7-8C5C-C20389284649}"/>
+    <hyperlink ref="B4" r:id="rId3" display="http://localhost:8084/survey-service/api/admin/survey" xr:uid="{6423608D-8AE5-4E50-AB5C-355ACED214A2}"/>
+    <hyperlink ref="B5" r:id="rId4" display="http://localhost:8084/survey-service/api/admin/survey/question " xr:uid="{CF357CFE-5953-4806-99F9-E22316F8537E}"/>
+    <hyperlink ref="B6" r:id="rId5" display="http://localhost:8084/survey-service/api/admin/survey/question " xr:uid="{2F48ED2F-AA4E-44F7-BA4C-AF5123711ED1}"/>
+    <hyperlink ref="B7" r:id="rId6" display="http://localhost:8084/survey-service/api/admin/survey/question " xr:uid="{BB3BA248-16F8-4DFB-8F70-32C138BE63E8}"/>
+    <hyperlink ref="B8" r:id="rId7" display="http://localhost:8084/survey-service/api/admin/survey" xr:uid="{6D7AA601-1E55-4774-A383-AD011F7648F2}"/>
+    <hyperlink ref="B9" r:id="rId8" display="http://localhost:8084/survey-service/api/admin/survey/question " xr:uid="{4884AE30-037E-4B3C-B54C-4F8009181292}"/>
+    <hyperlink ref="B10" r:id="rId9" display="http://localhost:8084/survey-service/api/customer/questionnaire" xr:uid="{D6BC5CF3-85EF-4326-9C61-3D922B6A0C80}"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://localhost:8084/survey-service/api/customer/questionnaire" xr:uid="{DA9FA8B0-3ED3-4714-B6B2-33F80A21E5A6}"/>
+    <hyperlink ref="B12" r:id="rId11" display="http://localhost:8084/survey-service/api/customer/questionnaire" xr:uid="{5D008E5D-70EC-460E-A3CB-414F5923E0C5}"/>
+    <hyperlink ref="B13" r:id="rId12" display="http://localhost:8084/survey-service/api/customer/questionnaire" xr:uid="{4D5DD549-A9F3-4D74-B1C2-69524B074915}"/>
+    <hyperlink ref="B14" r:id="rId13" display="http://localhost:8084/survey-service/api/customer/questionnaire" xr:uid="{2DB0D470-B447-4452-9645-55A854C29023}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>